<commit_message>
added script to configure winrm for ansible
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/azure_app_invoice.xlsx
+++ b/src/regionify/invoices/azure_app_invoice.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\preconfigured-apps\src\tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\git\preconfigured-apps\src\regionify\invoices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6720" yWindow="0" windowWidth="24000" windowHeight="9030"/>
+    <workbookView xWindow="7680" yWindow="0" windowWidth="24000" windowHeight="9030"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="45">
   <si>
     <t>OS</t>
   </si>
@@ -154,6 +154,12 @@
   </si>
   <si>
     <t>Red hat 7.2</t>
+  </si>
+  <si>
+    <t>Extension Script file</t>
+  </si>
+  <si>
+    <t>https://github.com/ansible/ansible/blob/devel/examples/scripts/ConfigureRemotingForAnsible.ps1</t>
   </si>
 </sst>
 </file>
@@ -239,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -257,6 +263,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,30 +578,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P6"/>
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:P6"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" customWidth="1"/>
-    <col min="4" max="6" width="17.28515625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15" customWidth="1"/>
-    <col min="13" max="13" width="14.85546875" customWidth="1"/>
-    <col min="14" max="14" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="5" max="7" width="17.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -602,283 +610,295 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>12</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>13</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>13</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>14</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="Q2" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>9</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>10</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>12</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>13</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>14</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="5" t="s">
+      <c r="N3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>20</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="Q3" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7"/>
+      <c r="D4" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>7.2</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>10</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>12</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>13</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>14</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>15</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N4" s="5" t="s">
+      <c r="O4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>20</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7"/>
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>7.2</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>10</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>13</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>14</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>15</v>
       </c>
-      <c r="M5" s="5" t="s">
+      <c r="N5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N5" s="5" t="s">
+      <c r="O5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>20</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="G6" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>10</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>12</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>13</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>14</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>15</v>
       </c>
-      <c r="M6" s="5" t="s">
+      <c r="N6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="N6" s="5" t="s">
+      <c r="O6" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>20</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated enable winrm script based on Evgeny's brew
</commit_message>
<xml_diff>
--- a/src/regionify/invoices/azure_app_invoice.xlsx
+++ b/src/regionify/invoices/azure_app_invoice.xlsx
@@ -159,13 +159,13 @@
     <t>Ubuntu 14</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/ansible/ansible/devel/examples/scripts/ConfigureRemotingForAnsible.ps1</t>
-  </si>
-  <si>
     <t>2016-Datacenter</t>
   </si>
   <si>
     <t>Windows Server 2016 Datacenter</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/QualiSystems/app-starter-pack/dev/scripts/enable-winrm.ps1</t>
   </si>
 </sst>
 </file>
@@ -586,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +670,7 @@
         <v>39</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>41</v>
@@ -717,10 +717,10 @@
     </row>
     <row r="3" spans="1:17" ht="16.5" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>46</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>44</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>41</v>
@@ -732,7 +732,7 @@
         <v>7</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H3" t="s">
         <v>9</v>

</xml_diff>